<commit_message>
syntax fixes in profile v0.2
</commit_message>
<xml_diff>
--- a/data/ciam_model_v6.xlsx
+++ b/data/ciam_model_v6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rstyczynski/projects/Crystal_IAM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8302D590-6D60-1A4C-AE0C-6F8240132896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76188B58-8267-6241-995D-ED88CA420C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{5ED2B057-FD68-AB4C-A7D6-457A64BE5DA0}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="228">
   <si>
     <t>OCI control plane privileges matrix</t>
   </si>
@@ -1459,10 +1459,10 @@
   <dimension ref="A1:CG234"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="14" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="14" topLeftCell="U41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -6296,7 +6296,9 @@
       <c r="X48" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="Y48" s="27"/>
+      <c r="Y48" s="27" t="s">
+        <v>10</v>
+      </c>
       <c r="Z48" s="27" t="s">
         <v>196</v>
       </c>
@@ -8360,7 +8362,7 @@
       </c>
       <c r="Y68" t="str">
         <f t="shared" si="20"/>
-        <v>ICORIIIPI</v>
+        <v>ICORIUIIPI</v>
       </c>
       <c r="Z68" t="str">
         <f t="shared" si="20"/>
@@ -10382,7 +10384,7 @@
       </c>
       <c r="Y74" t="str">
         <f t="shared" si="31"/>
-        <v>I</v>
+        <v>U</v>
       </c>
       <c r="Z74" t="str">
         <f t="shared" si="33"/>
@@ -11056,7 +11058,7 @@
       </c>
       <c r="Y76" t="str">
         <f t="shared" si="41"/>
-        <v>P</v>
+        <v>I</v>
       </c>
       <c r="Z76" t="str">
         <f t="shared" si="33"/>
@@ -11393,7 +11395,7 @@
       </c>
       <c r="Y77" t="str">
         <f t="shared" si="43"/>
-        <v>I</v>
+        <v>P</v>
       </c>
       <c r="Z77" t="str">
         <f t="shared" si="33"/>
@@ -11730,7 +11732,7 @@
       </c>
       <c r="Y78" t="str">
         <f t="shared" si="43"/>
-        <v/>
+        <v>I</v>
       </c>
       <c r="Z78" t="str">
         <f t="shared" si="33"/>
@@ -55876,7 +55878,7 @@
         <v>I</v>
       </c>
       <c r="Y209" s="33" t="str" cm="1">
-        <f t="array" ref="Y209:Y214">_xlfn.UNIQUE(Y69:Y208)</f>
+        <f t="array" ref="Y209:Y215">_xlfn.UNIQUE(Y69:Y208)</f>
         <v>I</v>
       </c>
       <c r="Z209" s="33" t="str" cm="1">
@@ -56680,7 +56682,7 @@
         <v>P</v>
       </c>
       <c r="Y213" s="33" t="str">
-        <v>P</v>
+        <v>U</v>
       </c>
       <c r="Z213" s="33" t="str">
         <v>P</v>
@@ -56829,7 +56831,7 @@
         <v/>
       </c>
       <c r="Y214" s="33" t="str">
-        <v/>
+        <v>P</v>
       </c>
       <c r="Z214" s="33" t="str">
         <v/>
@@ -56959,6 +56961,9 @@
       <c r="R215" s="33" t="str">
         <v/>
       </c>
+      <c r="Y215" s="33" t="str">
+        <v/>
+      </c>
       <c r="AE215" s="33" t="str">
         <v/>
       </c>
@@ -57787,7 +57792,7 @@
       </c>
       <c r="Y219" s="34" t="str">
         <f t="shared" si="235"/>
-        <v>U</v>
+        <v/>
       </c>
       <c r="Z219" s="34" t="str">
         <f t="shared" si="236"/>
@@ -59477,7 +59482,7 @@
       </c>
       <c r="Y225" s="6" t="str">
         <f t="shared" si="247"/>
-        <v>UDM</v>
+        <v>DM</v>
       </c>
       <c r="Z225" s="6" t="str">
         <f t="shared" si="247"/>

</xml_diff>

<commit_message>
service policies for object storage
</commit_message>
<xml_diff>
--- a/data/ciam_model_v6.xlsx
+++ b/data/ciam_model_v6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rstyczynski/projects/Crystal_IAM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEBD55F-5239-3F47-90D2-B97D570C59ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E92181-3285-BB48-9CDD-070208B33F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{5ED2B057-FD68-AB4C-A7D6-457A64BE5DA0}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="229">
   <si>
     <t>OCI control plane privileges matrix</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>Cloud Shell</t>
-  </si>
-  <si>
-    <t>object storage</t>
   </si>
   <si>
     <t>local network</t>
@@ -749,6 +746,9 @@
   </si>
   <si>
     <t>Network Path Analyzer</t>
+  </si>
+  <si>
+    <t>object storage / regionX|compartment cmp-security</t>
   </si>
 </sst>
 </file>
@@ -1462,10 +1462,10 @@
   <dimension ref="A1:CH234"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="14" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="14" topLeftCell="AX15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="L48" sqref="L48"/>
+      <selection pane="bottomRight" activeCell="BE14" sqref="BE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="2" spans="1:86" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:86" ht="44" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -1827,10 +1827,10 @@
     </row>
     <row r="7" spans="1:86" ht="22" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1921,15 +1921,15 @@
     </row>
     <row r="8" spans="1:86" ht="22" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="49" t="s">
         <v>171</v>
-      </c>
-      <c r="B8" s="49" t="s">
-        <v>172</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -2304,7 +2304,7 @@
         <v>Team</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D12" s="10" t="str">
         <f>C12</f>
@@ -2326,14 +2326,14 @@
         <v>Tenancy</v>
       </c>
       <c r="O12" s="48" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="P12" s="10" t="str">
         <f>O12</f>
         <v>Tenancy / info</v>
       </c>
       <c r="Q12" s="50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R12" s="50"/>
       <c r="S12" s="50"/>
@@ -2390,7 +2390,7 @@
         <v>Storage</v>
       </c>
       <c r="AR12" s="50" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AS12" s="50"/>
       <c r="AT12" s="10" t="str">
@@ -2398,7 +2398,7 @@
         <v>appgrp1 / Compute</v>
       </c>
       <c r="AU12" s="50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AV12" s="50"/>
       <c r="AW12" s="10" t="str">
@@ -2406,7 +2406,7 @@
         <v>appgrp1:Systems / Compute</v>
       </c>
       <c r="AX12" s="50" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AY12" s="50"/>
       <c r="AZ12" s="50"/>
@@ -2415,7 +2415,7 @@
         <v>appgrp1:Systems / Database</v>
       </c>
       <c r="BB12" s="50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="BC12" s="50"/>
       <c r="BD12" s="50"/>
@@ -2821,27 +2821,27 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:86" s="21" customFormat="1" ht="51" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:86" s="21" customFormat="1" ht="85" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J14" s="14" t="s">
         <v>36</v>
@@ -2850,194 +2850,194 @@
         <v>37</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M14" s="14" t="s">
         <v>38</v>
       </c>
       <c r="N14" s="14"/>
       <c r="O14" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P14" s="15"/>
       <c r="Q14" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R14" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="S14" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="S14" s="15" t="s">
-        <v>206</v>
-      </c>
       <c r="T14" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="U14" s="15"/>
       <c r="V14" s="16" t="s">
-        <v>39</v>
+        <v>228</v>
       </c>
       <c r="W14" s="16"/>
       <c r="X14" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y14" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="Y14" s="17" t="s">
+      <c r="Z14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="Z14" s="17" t="s">
+      <c r="AA14" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="AA14" s="17" t="s">
+      <c r="AB14" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC14" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AB14" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="AC14" s="17" t="s">
+      <c r="AD14" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="AD14" s="17" t="s">
-        <v>45</v>
       </c>
       <c r="AE14" s="17"/>
       <c r="AF14" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG14" s="18" t="s">
         <v>46</v>
-      </c>
-      <c r="AG14" s="18" t="s">
-        <v>47</v>
       </c>
       <c r="AH14" s="18"/>
       <c r="AI14" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ14" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="AJ14" s="18" t="s">
-        <v>49</v>
-      </c>
       <c r="AK14" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AL14" s="18"/>
       <c r="AM14" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN14" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="AN14" s="18" t="s">
+      <c r="AO14" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="AO14" s="18" t="s">
-        <v>52</v>
-      </c>
       <c r="AP14" s="18" t="s">
-        <v>39</v>
+        <v>228</v>
       </c>
       <c r="AQ14" s="18"/>
       <c r="AR14" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="AS14" s="17" t="s">
         <v>46</v>
-      </c>
-      <c r="AS14" s="17" t="s">
-        <v>47</v>
       </c>
       <c r="AT14" s="17"/>
       <c r="AU14" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV14" s="17" t="s">
         <v>46</v>
-      </c>
-      <c r="AV14" s="17" t="s">
-        <v>47</v>
       </c>
       <c r="AW14" s="17"/>
       <c r="AX14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="AY14" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="AY14" s="17" t="s">
-        <v>49</v>
-      </c>
       <c r="AZ14" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA14" s="17"/>
       <c r="BB14" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="BC14" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="BC14" s="17" t="s">
+      <c r="BD14" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="BD14" s="17" t="s">
-        <v>52</v>
-      </c>
       <c r="BE14" s="17" t="s">
-        <v>39</v>
+        <v>228</v>
       </c>
       <c r="BF14" s="17"/>
       <c r="BG14" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="BH14" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="BH14" s="19" t="s">
+      <c r="BI14" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="BI14" s="19" t="s">
+      <c r="BJ14" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="BK14" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="BJ14" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="BK14" s="19" t="s">
+      <c r="BL14" s="19" t="s">
         <v>56</v>
-      </c>
-      <c r="BL14" s="19" t="s">
-        <v>57</v>
       </c>
       <c r="BM14" s="19"/>
       <c r="BN14" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="BO14" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="BP14" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="BO14" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="BP14" s="16" t="s">
+      <c r="BQ14" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="BQ14" s="16" t="s">
+      <c r="BR14" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="BS14" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="BR14" s="16" t="s">
-        <v>199</v>
-      </c>
-      <c r="BS14" s="16" t="s">
+      <c r="BT14" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="BU14" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="BT14" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="BU14" s="16" t="s">
+      <c r="BV14" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="BW14" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="BV14" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="BW14" s="16" t="s">
-        <v>63</v>
-      </c>
       <c r="BX14" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BY14" s="16"/>
       <c r="BZ14" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="CA14" s="15" t="s">
         <v>64</v>
-      </c>
-      <c r="CA14" s="15" t="s">
-        <v>65</v>
       </c>
       <c r="CB14" s="15"/>
       <c r="CC14" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="CD14" s="14" t="s">
         <v>66</v>
-      </c>
-      <c r="CD14" s="14" t="s">
-        <v>67</v>
       </c>
       <c r="CE14" s="14"/>
       <c r="CF14" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="CG14" s="20" t="s">
         <v>68</v>
-      </c>
-      <c r="CG14" s="20" t="s">
-        <v>69</v>
       </c>
       <c r="CH14" s="20"/>
     </row>
@@ -3155,14 +3155,14 @@
     </row>
     <row r="16" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="24"/>
       <c r="F16" s="24" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
@@ -3253,7 +3253,7 @@
     </row>
     <row r="17" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="25"/>
@@ -3267,10 +3267,10 @@
         <v>14</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
@@ -3357,7 +3357,7 @@
     </row>
     <row r="18" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A18" s="47" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B18" s="23"/>
       <c r="C18" s="25"/>
@@ -3447,7 +3447,7 @@
     </row>
     <row r="19" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A19" s="47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="25"/>
@@ -3465,14 +3465,14 @@
       <c r="O19" s="25"/>
       <c r="P19" s="25"/>
       <c r="Q19" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R19" s="25"/>
       <c r="S19" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T19" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="U19" s="25"/>
       <c r="V19" s="26"/>
@@ -3543,7 +3543,7 @@
     </row>
     <row r="20" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A20" s="47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="23"/>
       <c r="C20" s="25"/>
@@ -3551,34 +3551,34 @@
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
       <c r="G20" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K20" s="24"/>
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
       <c r="N20" s="24"/>
       <c r="O20" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P20" s="25"/>
       <c r="Q20" s="25"/>
       <c r="R20" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="S20" s="25"/>
       <c r="T20" s="25"/>
       <c r="U20" s="25"/>
       <c r="V20" s="26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="W20" s="26"/>
       <c r="X20" s="27"/>
@@ -3647,7 +3647,7 @@
     </row>
     <row r="21" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B21" s="23"/>
       <c r="C21" s="25"/>
@@ -3670,7 +3670,7 @@
       <c r="T21" s="25"/>
       <c r="U21" s="25"/>
       <c r="V21" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="W21" s="26"/>
       <c r="X21" s="27"/>
@@ -3853,7 +3853,7 @@
     </row>
     <row r="23" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B23" s="23"/>
       <c r="C23" s="25"/>
@@ -3959,7 +3959,7 @@
     </row>
     <row r="24" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A24" s="47" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B24" s="23"/>
       <c r="C24" s="25"/>
@@ -4051,7 +4051,7 @@
     </row>
     <row r="25" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A25" s="47" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="25"/>
@@ -4147,7 +4147,7 @@
     </row>
     <row r="26" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A26" s="47" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="25"/>
@@ -4237,7 +4237,7 @@
     </row>
     <row r="27" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A27" s="47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="25"/>
@@ -4251,7 +4251,7 @@
       <c r="I27" s="24"/>
       <c r="J27" s="24"/>
       <c r="K27" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L27" s="24" t="s">
         <v>10</v>
@@ -4339,7 +4339,7 @@
     </row>
     <row r="28" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A28" s="47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="23"/>
       <c r="C28" s="25"/>
@@ -4366,7 +4366,7 @@
       <c r="X28" s="27"/>
       <c r="Y28" s="27"/>
       <c r="Z28" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AA28" s="27"/>
       <c r="AB28" s="27"/>
@@ -4431,7 +4431,7 @@
     </row>
     <row r="29" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A29" s="47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B29" s="23"/>
       <c r="C29" s="25"/>
@@ -4511,23 +4511,23 @@
       <c r="BY29" s="26"/>
       <c r="BZ29" s="25"/>
       <c r="CA29" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="CB29" s="25"/>
       <c r="CC29" s="24"/>
       <c r="CD29" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="CE29" s="24"/>
       <c r="CF29" s="30"/>
       <c r="CG29" s="30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="CH29" s="30"/>
     </row>
     <row r="30" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A30" s="47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" s="23"/>
       <c r="C30" s="25"/>
@@ -4619,7 +4619,7 @@
     </row>
     <row r="31" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B31" s="23"/>
       <c r="C31" s="25"/>
@@ -4709,7 +4709,7 @@
     </row>
     <row r="32" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A32" s="47" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="25"/>
@@ -4823,11 +4823,11 @@
     </row>
     <row r="33" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A33" s="47" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B33" s="23"/>
       <c r="C33" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D33" s="25"/>
       <c r="E33" s="24"/>
@@ -4929,7 +4929,7 @@
     </row>
     <row r="34" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A34" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" s="23"/>
       <c r="C34" s="25"/>
@@ -5027,7 +5027,7 @@
     </row>
     <row r="35" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A35" s="47" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="25"/>
@@ -5129,7 +5129,7 @@
     </row>
     <row r="36" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A36" s="47" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B36" s="23"/>
       <c r="C36" s="25"/>
@@ -5235,7 +5235,7 @@
     </row>
     <row r="37" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A37" s="47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B37" s="23"/>
       <c r="C37" s="25"/>
@@ -5337,7 +5337,7 @@
     </row>
     <row r="38" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A38" s="47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B38" s="23"/>
       <c r="C38" s="25"/>
@@ -5433,7 +5433,7 @@
     </row>
     <row r="39" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A39" s="47" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B39" s="23"/>
       <c r="C39" s="25"/>
@@ -5527,7 +5527,7 @@
     </row>
     <row r="40" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A40" s="47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B40" s="23"/>
       <c r="C40" s="25"/>
@@ -5621,7 +5621,7 @@
     </row>
     <row r="41" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B41" s="23"/>
       <c r="C41" s="25"/>
@@ -5711,7 +5711,7 @@
     </row>
     <row r="42" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B42" s="23"/>
       <c r="C42" s="25"/>
@@ -5751,10 +5751,10 @@
       <c r="AG42" s="28"/>
       <c r="AH42" s="28"/>
       <c r="AI42" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AJ42" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AK42" s="28"/>
       <c r="AL42" s="28"/>
@@ -5770,10 +5770,10 @@
       <c r="AV42" s="27"/>
       <c r="AW42" s="27"/>
       <c r="AX42" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AY42" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AZ42" s="27"/>
       <c r="BA42" s="27"/>
@@ -5813,7 +5813,7 @@
     </row>
     <row r="43" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A43" s="47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B43" s="23"/>
       <c r="C43" s="25"/>
@@ -5855,7 +5855,7 @@
       <c r="AI43" s="28"/>
       <c r="AJ43" s="28"/>
       <c r="AK43" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AL43" s="28"/>
       <c r="AM43" s="28"/>
@@ -5872,7 +5872,7 @@
       <c r="AX43" s="27"/>
       <c r="AY43" s="27"/>
       <c r="AZ43" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BA43" s="27"/>
       <c r="BB43" s="27"/>
@@ -5911,7 +5911,7 @@
     </row>
     <row r="44" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A44" s="47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B44" s="23"/>
       <c r="C44" s="25"/>
@@ -5948,10 +5948,10 @@
       <c r="AD44" s="27"/>
       <c r="AE44" s="27"/>
       <c r="AF44" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AG44" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AH44" s="28"/>
       <c r="AI44" s="28"/>
@@ -5970,17 +5970,17 @@
       <c r="AP44" s="28"/>
       <c r="AQ44" s="28"/>
       <c r="AR44" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AS44" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AT44" s="27"/>
       <c r="AU44" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AV44" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AW44" s="27"/>
       <c r="AX44" s="27"/>
@@ -6029,7 +6029,7 @@
     </row>
     <row r="45" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A45" s="47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" s="23"/>
       <c r="C45" s="25"/>
@@ -6056,7 +6056,7 @@
       <c r="T45" s="25"/>
       <c r="U45" s="25"/>
       <c r="V45" s="26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="W45" s="26"/>
       <c r="X45" s="27"/>
@@ -6075,14 +6075,14 @@
       <c r="AK45" s="28"/>
       <c r="AL45" s="28"/>
       <c r="AM45" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AN45" s="28"/>
       <c r="AO45" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP45" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AQ45" s="28"/>
       <c r="AR45" s="27"/>
@@ -6096,14 +6096,14 @@
       <c r="AZ45" s="27"/>
       <c r="BA45" s="27"/>
       <c r="BB45" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BC45" s="27"/>
       <c r="BD45" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BE45" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BF45" s="27"/>
       <c r="BG45" s="29"/>
@@ -6137,7 +6137,7 @@
     </row>
     <row r="46" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A46" s="47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="23"/>
       <c r="C46" s="25"/>
@@ -6182,7 +6182,7 @@
       <c r="AL46" s="28"/>
       <c r="AM46" s="28"/>
       <c r="AN46" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO46" s="28"/>
       <c r="AP46" s="28"/>
@@ -6199,7 +6199,7 @@
       <c r="BA46" s="27"/>
       <c r="BB46" s="27"/>
       <c r="BC46" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BD46" s="27"/>
       <c r="BE46" s="27"/>
@@ -6235,7 +6235,7 @@
     </row>
     <row r="47" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A47" s="47" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B47" s="23"/>
       <c r="C47" s="25"/>
@@ -6325,7 +6325,7 @@
     </row>
     <row r="48" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A48" s="47" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B48" s="23"/>
       <c r="C48" s="25"/>
@@ -6349,28 +6349,30 @@
       <c r="S48" s="25"/>
       <c r="T48" s="25"/>
       <c r="U48" s="25"/>
-      <c r="V48" s="26"/>
+      <c r="V48" s="26" t="s">
+        <v>10</v>
+      </c>
       <c r="W48" s="26"/>
       <c r="X48" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Y48" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Z48" s="27" t="s">
         <v>10</v>
       </c>
       <c r="AA48" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AB48" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AC48" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AD48" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AE48" s="27"/>
       <c r="AF48" s="28"/>
@@ -6431,7 +6433,7 @@
     </row>
     <row r="49" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A49" s="47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B49" s="23"/>
       <c r="C49" s="25"/>
@@ -6510,7 +6512,7 @@
       <c r="BX49" s="26"/>
       <c r="BY49" s="26"/>
       <c r="BZ49" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="CA49" s="25"/>
       <c r="CB49" s="25"/>
@@ -6523,7 +6525,7 @@
     </row>
     <row r="50" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A50" s="47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B50" s="23"/>
       <c r="C50" s="25"/>
@@ -6605,7 +6607,7 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="25"/>
       <c r="CC50" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="CD50" s="24"/>
       <c r="CE50" s="24"/>
@@ -6615,7 +6617,7 @@
     </row>
     <row r="51" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A51" s="47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B51" s="23"/>
       <c r="C51" s="25"/>
@@ -6700,14 +6702,14 @@
       <c r="CD51" s="24"/>
       <c r="CE51" s="24"/>
       <c r="CF51" s="30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="CG51" s="30"/>
       <c r="CH51" s="30"/>
     </row>
     <row r="52" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B52" s="23"/>
       <c r="C52" s="25"/>
@@ -6797,7 +6799,7 @@
     </row>
     <row r="53" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A53" s="47" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B53" s="23"/>
       <c r="C53" s="25"/>
@@ -6969,7 +6971,7 @@
     </row>
     <row r="54" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A54" s="47" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B54" s="23"/>
       <c r="C54" s="25"/>
@@ -7059,7 +7061,7 @@
     </row>
     <row r="55" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A55" s="47" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B55" s="23"/>
       <c r="C55" s="25"/>
@@ -7173,18 +7175,18 @@
       </c>
       <c r="BF55" s="27"/>
       <c r="BG55" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BH55" s="29" t="s">
         <v>14</v>
       </c>
       <c r="BI55" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BJ55" s="29"/>
       <c r="BK55" s="29"/>
       <c r="BL55" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BM55" s="29"/>
       <c r="BN55" s="26" t="s">
@@ -7231,7 +7233,7 @@
     </row>
     <row r="56" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B56" s="23"/>
       <c r="C56" s="25"/>
@@ -7321,7 +7323,7 @@
     </row>
     <row r="57" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A57" s="46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B57" s="23"/>
       <c r="C57" s="25"/>
@@ -7465,7 +7467,7 @@
     </row>
     <row r="58" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A58" s="46" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B58" s="23"/>
       <c r="C58" s="25"/>
@@ -7625,7 +7627,7 @@
     </row>
     <row r="59" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A59" s="46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B59" s="23"/>
       <c r="C59" s="25"/>
@@ -7719,7 +7721,7 @@
     </row>
     <row r="60" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A60" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B60" s="23"/>
       <c r="C60" s="25"/>
@@ -7809,7 +7811,7 @@
     </row>
     <row r="61" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A61" s="47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B61" s="23"/>
       <c r="C61" s="25"/>
@@ -7905,7 +7907,7 @@
     </row>
     <row r="62" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A62" s="47" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B62" s="23"/>
       <c r="C62" s="25"/>
@@ -7999,7 +8001,7 @@
     </row>
     <row r="63" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A63" s="47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B63" s="23"/>
       <c r="C63" s="25"/>
@@ -8091,7 +8093,7 @@
     </row>
     <row r="64" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A64" s="47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B64" s="23"/>
       <c r="C64" s="25"/>
@@ -8197,7 +8199,7 @@
     </row>
     <row r="65" spans="1:86" s="5" customFormat="1" ht="22" x14ac:dyDescent="0.25">
       <c r="A65" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B65" s="23"/>
       <c r="C65" s="25"/>
@@ -8432,7 +8434,7 @@
       </c>
       <c r="V68" t="str">
         <f t="shared" si="20"/>
-        <v>UCORUICORII</v>
+        <v>UCORUICORUII</v>
       </c>
       <c r="W68" t="str">
         <f t="shared" si="20"/>
@@ -11842,7 +11844,7 @@
       </c>
       <c r="V78" t="str">
         <f t="shared" si="44"/>
-        <v>I</v>
+        <v>U</v>
       </c>
       <c r="W78" t="str">
         <f t="shared" si="44"/>
@@ -12524,7 +12526,7 @@
       </c>
       <c r="V80" t="str">
         <f t="shared" si="44"/>
-        <v/>
+        <v>I</v>
       </c>
       <c r="W80" t="str">
         <f t="shared" si="44"/>
@@ -58708,7 +58710,7 @@
     </row>
     <row r="220" spans="2:86" s="34" customFormat="1" ht="22" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B220" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C220" s="34" t="str">
         <f t="shared" si="231"/>
@@ -59049,7 +59051,7 @@
     </row>
     <row r="221" spans="2:86" s="34" customFormat="1" ht="22" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B221" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C221" s="34" t="str">
         <f t="shared" si="231"/>
@@ -60077,7 +60079,7 @@
     </row>
     <row r="225" spans="1:86" s="5" customFormat="1" ht="46" customHeight="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A225" s="35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C225" s="6" t="str">
         <f t="shared" ref="C225:D225" si="247">IF(C14&lt;&gt;"",IF(_xlfn.TEXTJOIN("",TRUE,C217:C224)="","(ok)",_xlfn.TEXTJOIN("",TRUE,C217:C224)),"")</f>
@@ -60512,10 +60514,10 @@
         <v>33</v>
       </c>
       <c r="B1" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>100</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -60523,10 +60525,10 @@
         <v>29</v>
       </c>
       <c r="B2" s="42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="42" t="s">
         <v>102</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60534,10 +60536,10 @@
         <v>29</v>
       </c>
       <c r="B3" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="42" t="s">
         <v>104</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60545,10 +60547,10 @@
         <v>29</v>
       </c>
       <c r="B4" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="42" t="s">
         <v>106</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60556,10 +60558,10 @@
         <v>29</v>
       </c>
       <c r="B5" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="42" t="s">
         <v>108</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60567,10 +60569,10 @@
         <v>29</v>
       </c>
       <c r="B6" s="42" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="42" t="s">
         <v>110</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -60578,10 +60580,10 @@
         <v>29</v>
       </c>
       <c r="B7" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="42" t="s">
         <v>112</v>
-      </c>
-      <c r="C7" s="42" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -60594,10 +60596,10 @@
         <v>33</v>
       </c>
       <c r="B9" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="40" t="s">
         <v>100</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -60605,10 +60607,10 @@
         <v>23</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60616,10 +60618,10 @@
         <v>23</v>
       </c>
       <c r="B11" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="42" t="s">
         <v>115</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60627,10 +60629,10 @@
         <v>23</v>
       </c>
       <c r="B12" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="42" t="s">
         <v>117</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60638,10 +60640,10 @@
         <v>23</v>
       </c>
       <c r="B13" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="42" t="s">
         <v>119</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60652,7 +60654,7 @@
         <v>35</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="35" thickBot="1" x14ac:dyDescent="0.25">
@@ -60663,7 +60665,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60671,10 +60673,10 @@
         <v>23</v>
       </c>
       <c r="B16" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="42" t="s">
         <v>123</v>
-      </c>
-      <c r="C16" s="42" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -60687,65 +60689,65 @@
         <v>33</v>
       </c>
       <c r="B18" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="40" t="s">
         <v>100</v>
-      </c>
-      <c r="C18" s="40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="42" t="s">
         <v>125</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="42" t="s">
         <v>127</v>
-      </c>
-      <c r="C20" s="42" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B21" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="42" t="s">
         <v>129</v>
-      </c>
-      <c r="C21" s="42" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="42" t="s">
         <v>131</v>
-      </c>
-      <c r="C22" s="42" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" s="42" t="s">
         <v>133</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -60758,10 +60760,10 @@
         <v>33</v>
       </c>
       <c r="B25" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="40" t="s">
         <v>100</v>
-      </c>
-      <c r="C25" s="40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -60769,10 +60771,10 @@
         <v>27</v>
       </c>
       <c r="B26" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="42" t="s">
         <v>135</v>
-      </c>
-      <c r="C26" s="42" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60780,10 +60782,10 @@
         <v>27</v>
       </c>
       <c r="B27" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="C27" s="42" t="s">
         <v>137</v>
-      </c>
-      <c r="C27" s="42" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60791,10 +60793,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -60807,10 +60809,10 @@
         <v>33</v>
       </c>
       <c r="B30" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="40" t="s">
         <v>100</v>
-      </c>
-      <c r="C30" s="40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -60818,10 +60820,10 @@
         <v>24</v>
       </c>
       <c r="B31" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="42" t="s">
         <v>140</v>
-      </c>
-      <c r="C31" s="42" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60829,10 +60831,10 @@
         <v>24</v>
       </c>
       <c r="B32" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="C32" s="42" t="s">
         <v>142</v>
-      </c>
-      <c r="C32" s="42" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -60840,10 +60842,10 @@
         <v>24</v>
       </c>
       <c r="B33" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33" s="42" t="s">
         <v>144</v>
-      </c>
-      <c r="C33" s="42" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -60856,32 +60858,32 @@
         <v>33</v>
       </c>
       <c r="B35" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="40" t="s">
         <v>100</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B36" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" s="42" t="s">
         <v>146</v>
-      </c>
-      <c r="C36" s="42" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B37" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="42" t="s">
         <v>148</v>
-      </c>
-      <c r="C37" s="42" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -60894,43 +60896,43 @@
         <v>33</v>
       </c>
       <c r="B39" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="40" t="s">
         <v>100</v>
-      </c>
-      <c r="C39" s="40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B40" s="42" t="s">
         <v>28</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B41" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41" s="42" t="s">
         <v>152</v>
-      </c>
-      <c r="C41" s="42" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B42" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42" s="42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -60943,76 +60945,76 @@
         <v>33</v>
       </c>
       <c r="B44" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="40" t="s">
         <v>100</v>
-      </c>
-      <c r="C44" s="40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B45" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" s="42" t="s">
         <v>155</v>
-      </c>
-      <c r="C45" s="42" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B46" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C46" s="42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B47" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="C47" s="42" t="s">
         <v>158</v>
-      </c>
-      <c r="C47" s="42" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="42" t="s">
         <v>155</v>
-      </c>
-      <c r="C48" s="42" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B49" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="C50" s="42" t="s">
         <v>160</v>
-      </c>
-      <c r="C50" s="42" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -61025,43 +61027,43 @@
         <v>33</v>
       </c>
       <c r="B52" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="40" t="s">
         <v>100</v>
-      </c>
-      <c r="C52" s="40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B53" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" s="42" t="s">
         <v>155</v>
-      </c>
-      <c r="C53" s="42" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B54" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="B55" s="42" t="s">
+      <c r="C55" s="42" t="s">
         <v>163</v>
-      </c>
-      <c r="C55" s="42" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -61074,32 +61076,32 @@
         <v>33</v>
       </c>
       <c r="B57" s="40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="40" t="s">
         <v>100</v>
-      </c>
-      <c r="C57" s="40" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B58" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="C58" s="42" t="s">
         <v>165</v>
-      </c>
-      <c r="C58" s="42" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="B59" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="B59" s="42" t="s">
+      <c r="C59" s="42" t="s">
         <v>168</v>
-      </c>
-      <c r="C59" s="42" t="s">
-        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PT50|Update service access for services (after CIS LZ)
</commit_message>
<xml_diff>
--- a/data/ciam_model_v6.xlsx
+++ b/data/ciam_model_v6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rstyczynski/projects/Crystal_IAM/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E92181-3285-BB48-9CDD-070208B33F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F91DBA-E2D7-EB48-9230-AF548F0F4FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="760" windowWidth="30240" windowHeight="17620" xr2:uid="{5ED2B057-FD68-AB4C-A7D6-457A64BE5DA0}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="230">
   <si>
     <t>OCI control plane privileges matrix</t>
   </si>
@@ -749,6 +749,9 @@
   </si>
   <si>
     <t>object storage / regionX|compartment cmp-security</t>
+  </si>
+  <si>
+    <t>kubernetes / compartment cmp-security</t>
   </si>
 </sst>
 </file>
@@ -1462,10 +1465,10 @@
   <dimension ref="A1:CH234"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="14" topLeftCell="AX15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="14" topLeftCell="AR15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="BE14" sqref="BE14"/>
+      <selection pane="bottomRight" activeCell="AV15" sqref="AV15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2940,7 +2943,7 @@
         <v>45</v>
       </c>
       <c r="AV14" s="17" t="s">
-        <v>46</v>
+        <v>229</v>
       </c>
       <c r="AW14" s="17"/>
       <c r="AX14" s="17" t="s">

</xml_diff>